<commit_message>
saving before changing to 32-bit data bus
</commit_message>
<xml_diff>
--- a/HW2/autogen/CUSignals.xlsx
+++ b/HW2/autogen/CUSignals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW2\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A88F62B-90F0-4836-A960-2D8BB06F1012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199141D6-5FDD-4BE5-A86F-67CCC6BAD855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3355" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="264">
   <si>
     <t>Instruction</t>
   </si>
@@ -841,6 +841,9 @@
       <t>ASel</t>
     </r>
   </si>
+  <si>
+    <t>DBOutSel_Result</t>
+  </si>
 </sst>
 </file>
 
@@ -1510,7 +1513,7 @@
   </sheetPr>
   <dimension ref="A1:AF124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A127" sqref="A127"/>
     </sheetView>
@@ -14961,11 +14964,11 @@
       </c>
       <c r="N104" s="18" t="str">
         <f>DAU!B104</f>
-        <v>unused</v>
+        <v>DAU_AddrRn</v>
       </c>
       <c r="O104" s="18" t="str">
         <f>DAU!C104</f>
-        <v>unused</v>
+        <v>DAU_OffsetZero</v>
       </c>
       <c r="P104" s="17" t="str">
         <f>DAU!D104</f>
@@ -15007,9 +15010,9 @@
         <f>REG!G104</f>
         <v>0</v>
       </c>
-      <c r="Z104" s="17">
+      <c r="Z104" s="17" t="str">
         <f>REG!H104</f>
-        <v>0</v>
+        <v>RegASelCmd_Rn</v>
       </c>
       <c r="AA104" s="17">
         <f>REG!I104</f>
@@ -15091,11 +15094,11 @@
       </c>
       <c r="N105" s="18" t="str">
         <f>DAU!B105</f>
-        <v>unused</v>
+        <v>DAU_AddrRn</v>
       </c>
       <c r="O105" s="18" t="str">
         <f>DAU!C105</f>
-        <v>unused</v>
+        <v>DAU_OffsetZero</v>
       </c>
       <c r="P105" s="17" t="str">
         <f>DAU!D105</f>
@@ -15137,9 +15140,9 @@
         <f>REG!G105</f>
         <v>0</v>
       </c>
-      <c r="Z105" s="17">
+      <c r="Z105" s="17" t="str">
         <f>REG!H105</f>
-        <v>0</v>
+        <v>RegASelCmd_Rn</v>
       </c>
       <c r="AA105" s="17">
         <f>REG!I105</f>
@@ -15221,11 +15224,11 @@
       </c>
       <c r="N106" s="18" t="str">
         <f>DAU!B106</f>
-        <v>unused</v>
+        <v>DAU_AddrRn</v>
       </c>
       <c r="O106" s="18" t="str">
         <f>DAU!C106</f>
-        <v>unused</v>
+        <v>DAU_OffsetZero</v>
       </c>
       <c r="P106" s="17" t="str">
         <f>DAU!D106</f>
@@ -15267,9 +15270,9 @@
         <f>REG!G106</f>
         <v>0</v>
       </c>
-      <c r="Z106" s="17">
+      <c r="Z106" s="17" t="str">
         <f>REG!H106</f>
-        <v>0</v>
+        <v>RegASelCmd_Rn</v>
       </c>
       <c r="AA106" s="17">
         <f>REG!I106</f>
@@ -17651,8 +17654,8 @@
   </sheetPr>
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23413,7 +23416,9 @@
   </sheetPr>
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25780,10 +25785,10 @@
         <v>110</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="D104" s="18" t="s">
         <v>164</v>
@@ -25803,10 +25808,10 @@
         <v>111</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="D105" s="18" t="s">
         <v>164</v>
@@ -25826,10 +25831,10 @@
         <v>112</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="D106" s="18" t="s">
         <v>164</v>
@@ -26269,7 +26274,9 @@
   </sheetPr>
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29557,7 +29564,9 @@
       <c r="D103" s="18"/>
       <c r="E103" s="18"/>
       <c r="F103" s="18"/>
-      <c r="G103" s="25"/>
+      <c r="G103" s="25">
+        <v>0</v>
+      </c>
       <c r="H103" s="18"/>
       <c r="I103" s="18"/>
       <c r="J103" s="19" t="s">
@@ -29573,8 +29582,12 @@
       <c r="D104" s="18"/>
       <c r="E104" s="18"/>
       <c r="F104" s="18"/>
-      <c r="G104" s="25"/>
-      <c r="H104" s="19"/>
+      <c r="G104" s="25">
+        <v>0</v>
+      </c>
+      <c r="H104" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="I104" s="19"/>
       <c r="J104" s="19" t="s">
         <v>150</v>
@@ -29589,8 +29602,12 @@
       <c r="D105" s="18"/>
       <c r="E105" s="18"/>
       <c r="F105" s="18"/>
-      <c r="G105" s="25"/>
-      <c r="H105" s="19"/>
+      <c r="G105" s="25">
+        <v>0</v>
+      </c>
+      <c r="H105" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="I105" s="19"/>
       <c r="J105" s="19" t="s">
         <v>150</v>
@@ -29605,8 +29622,12 @@
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
       <c r="F106" s="18"/>
-      <c r="G106" s="25"/>
-      <c r="H106" s="19"/>
+      <c r="G106" s="25">
+        <v>0</v>
+      </c>
+      <c r="H106" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="I106" s="19"/>
       <c r="J106" s="19" t="s">
         <v>150</v>
@@ -29621,7 +29642,9 @@
       <c r="D107" s="18"/>
       <c r="E107" s="20"/>
       <c r="F107" s="19"/>
-      <c r="G107" s="25"/>
+      <c r="G107" s="25">
+        <v>0</v>
+      </c>
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
       <c r="J107" s="19" t="s">
@@ -29637,7 +29660,9 @@
       <c r="D108" s="18"/>
       <c r="E108" s="20"/>
       <c r="F108" s="19"/>
-      <c r="G108" s="25"/>
+      <c r="G108" s="25">
+        <v>0</v>
+      </c>
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
       <c r="J108" s="19" t="s">
@@ -29653,7 +29678,9 @@
       <c r="D109" s="18"/>
       <c r="E109" s="20"/>
       <c r="F109" s="19"/>
-      <c r="G109" s="25"/>
+      <c r="G109" s="25">
+        <v>0</v>
+      </c>
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
       <c r="J109" s="19" t="s">
@@ -29669,7 +29696,9 @@
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
       <c r="F110" s="18"/>
-      <c r="G110" s="25"/>
+      <c r="G110" s="25">
+        <v>0</v>
+      </c>
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
       <c r="J110" s="19" t="s">
@@ -29685,7 +29714,9 @@
       <c r="D111" s="18"/>
       <c r="E111" s="20"/>
       <c r="F111" s="19"/>
-      <c r="G111" s="25"/>
+      <c r="G111" s="25">
+        <v>0</v>
+      </c>
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
       <c r="J111" s="19" t="s">
@@ -29701,7 +29732,9 @@
       <c r="D112" s="18"/>
       <c r="E112" s="18"/>
       <c r="F112" s="18"/>
-      <c r="G112" s="25"/>
+      <c r="G112" s="25">
+        <v>0</v>
+      </c>
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
       <c r="J112" s="19" t="s">
@@ -29717,7 +29750,9 @@
       <c r="D113" s="20"/>
       <c r="E113" s="20"/>
       <c r="F113" s="19"/>
-      <c r="G113" s="25"/>
+      <c r="G113" s="25">
+        <v>0</v>
+      </c>
       <c r="H113" s="19"/>
       <c r="I113" s="19"/>
       <c r="J113" s="19" t="s">
@@ -29733,7 +29768,9 @@
       <c r="D114" s="18"/>
       <c r="E114" s="18"/>
       <c r="F114" s="18"/>
-      <c r="G114" s="25"/>
+      <c r="G114" s="25">
+        <v>0</v>
+      </c>
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
       <c r="J114" s="19" t="s">
@@ -29749,7 +29786,9 @@
       <c r="D115" s="18"/>
       <c r="E115" s="18"/>
       <c r="F115" s="18"/>
-      <c r="G115" s="25"/>
+      <c r="G115" s="25">
+        <v>0</v>
+      </c>
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
       <c r="J115" s="19" t="s">
@@ -29765,7 +29804,9 @@
       <c r="D116" s="18"/>
       <c r="E116" s="18"/>
       <c r="F116" s="18"/>
-      <c r="G116" s="25"/>
+      <c r="G116" s="25">
+        <v>0</v>
+      </c>
       <c r="H116" s="19"/>
       <c r="I116" s="19"/>
       <c r="J116" s="19" t="s">
@@ -29781,7 +29822,9 @@
       <c r="D117" s="18"/>
       <c r="E117" s="18"/>
       <c r="F117" s="18"/>
-      <c r="G117" s="25"/>
+      <c r="G117" s="25">
+        <v>0</v>
+      </c>
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>
       <c r="J117" s="19" t="s">
@@ -29797,7 +29840,9 @@
       <c r="D118" s="18"/>
       <c r="E118" s="20"/>
       <c r="F118" s="19"/>
-      <c r="G118" s="25"/>
+      <c r="G118" s="25">
+        <v>0</v>
+      </c>
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
       <c r="J118" s="19" t="s">
@@ -29813,7 +29858,9 @@
       <c r="D119" s="18"/>
       <c r="E119" s="20"/>
       <c r="F119" s="19"/>
-      <c r="G119" s="25"/>
+      <c r="G119" s="25">
+        <v>0</v>
+      </c>
       <c r="H119" s="19"/>
       <c r="I119" s="19"/>
       <c r="J119" s="19" t="s">
@@ -29829,7 +29876,9 @@
       <c r="D120" s="18"/>
       <c r="E120" s="20"/>
       <c r="F120" s="19"/>
-      <c r="G120" s="25"/>
+      <c r="G120" s="25">
+        <v>0</v>
+      </c>
       <c r="H120" s="19"/>
       <c r="I120" s="19"/>
       <c r="J120" s="19" t="s">
@@ -29845,7 +29894,9 @@
       <c r="D121" s="18"/>
       <c r="E121" s="18"/>
       <c r="F121" s="18"/>
-      <c r="G121" s="25"/>
+      <c r="G121" s="25">
+        <v>0</v>
+      </c>
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
       <c r="J121" s="19" t="s">
@@ -29861,7 +29912,9 @@
       <c r="D122" s="18"/>
       <c r="E122" s="20"/>
       <c r="F122" s="19"/>
-      <c r="G122" s="25"/>
+      <c r="G122" s="25">
+        <v>0</v>
+      </c>
       <c r="H122" s="19"/>
       <c r="I122" s="19"/>
       <c r="J122" s="19" t="s">
@@ -29877,7 +29930,9 @@
       <c r="D123" s="18"/>
       <c r="E123" s="20"/>
       <c r="F123" s="19"/>
-      <c r="G123" s="25"/>
+      <c r="G123" s="25">
+        <v>0</v>
+      </c>
       <c r="H123" s="19"/>
       <c r="I123" s="19"/>
       <c r="J123" s="19" t="s">
@@ -29887,6 +29942,9 @@
     <row r="124" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>133</v>
+      </c>
+      <c r="G124" s="25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -29904,7 +29962,9 @@
   </sheetPr>
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29952,7 +30012,9 @@
       <c r="C2" s="17">
         <v>0</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19"/>
@@ -29963,7 +30025,7 @@
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="B3" s="17">
         <v>1</v>
@@ -29971,7 +30033,9 @@
       <c r="C3" s="17">
         <v>0</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
@@ -29982,7 +30046,7 @@
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="B4" s="17">
         <v>1</v>
@@ -29990,7 +30054,9 @@
       <c r="C4" s="17">
         <v>0</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
@@ -30009,7 +30075,9 @@
       <c r="C5" s="17">
         <v>0</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -30028,7 +30096,9 @@
       <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
@@ -30047,7 +30117,9 @@
       <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="19"/>
@@ -30066,7 +30138,9 @@
       <c r="C8" s="17">
         <v>1</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
@@ -30085,7 +30159,9 @@
       <c r="C9" s="17">
         <v>0</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
@@ -30104,7 +30180,9 @@
       <c r="C10" s="17">
         <v>0</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
@@ -30123,7 +30201,9 @@
       <c r="C11" s="17">
         <v>0</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
@@ -30142,7 +30222,9 @@
       <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="20"/>
       <c r="G12" s="19"/>
@@ -30161,7 +30243,9 @@
       <c r="C13" s="17">
         <v>1</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="20"/>
       <c r="G13" s="19"/>
@@ -30180,7 +30264,9 @@
       <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
@@ -30199,7 +30285,9 @@
       <c r="C15" s="17">
         <v>0</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E15" s="18"/>
       <c r="F15" s="20"/>
       <c r="G15" s="19"/>
@@ -30218,7 +30306,9 @@
       <c r="C16" s="17">
         <v>0</v>
       </c>
-      <c r="D16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E16" s="18"/>
       <c r="F16" s="20"/>
       <c r="G16" s="19"/>
@@ -30237,7 +30327,9 @@
       <c r="C17" s="17">
         <v>0</v>
       </c>
-      <c r="D17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E17" s="18"/>
       <c r="F17" s="20"/>
       <c r="G17" s="19"/>
@@ -30256,7 +30348,9 @@
       <c r="C18" s="17">
         <v>1</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="19"/>
@@ -30275,7 +30369,9 @@
       <c r="C19" s="17">
         <v>1</v>
       </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="19"/>
@@ -30294,7 +30390,9 @@
       <c r="C20" s="17">
         <v>1</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="19"/>
@@ -30313,7 +30411,9 @@
       <c r="C21" s="17">
         <v>0</v>
       </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
@@ -30332,7 +30432,9 @@
       <c r="C22" s="17">
         <v>0</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="19"/>
@@ -30351,7 +30453,9 @@
       <c r="C23" s="17">
         <v>0</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="19"/>
@@ -30370,7 +30474,9 @@
       <c r="C24" s="17">
         <v>1</v>
       </c>
-      <c r="D24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
@@ -30389,7 +30495,9 @@
       <c r="C25" s="17">
         <v>1</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
@@ -30408,7 +30516,9 @@
       <c r="C26" s="17">
         <v>1</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="19"/>
@@ -30427,7 +30537,9 @@
       <c r="C27" s="17">
         <v>0</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
@@ -30446,7 +30558,9 @@
       <c r="C28" s="17">
         <v>0</v>
       </c>
-      <c r="D28" s="17"/>
+      <c r="D28" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="19"/>
@@ -30465,7 +30579,9 @@
       <c r="C29" s="17">
         <v>0</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="19"/>
@@ -30484,7 +30600,9 @@
       <c r="C30" s="17">
         <v>1</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="19"/>
@@ -30503,7 +30621,9 @@
       <c r="C31" s="17">
         <v>1</v>
       </c>
-      <c r="D31" s="17"/>
+      <c r="D31" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="19"/>
@@ -30522,7 +30642,9 @@
       <c r="C32" s="17">
         <v>1</v>
       </c>
-      <c r="D32" s="17"/>
+      <c r="D32" s="17" t="s">
+        <v>263</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="19"/>
@@ -30541,7 +30663,9 @@
       <c r="C33" s="17">
         <v>0</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="19"/>
@@ -30560,7 +30684,9 @@
       <c r="C34" s="17">
         <v>0</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="19"/>
@@ -30579,7 +30705,9 @@
       <c r="C35" s="17">
         <v>0</v>
       </c>
-      <c r="D35" s="17"/>
+      <c r="D35" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="19"/>
@@ -30693,7 +30821,9 @@
       <c r="C41" s="17">
         <v>0</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E41" s="19"/>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
@@ -30712,7 +30842,9 @@
       <c r="C42" s="17">
         <v>0</v>
       </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E42" s="19"/>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
@@ -30731,7 +30863,9 @@
       <c r="C43" s="17">
         <v>0</v>
       </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E43" s="19"/>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
@@ -30750,7 +30884,9 @@
       <c r="C44" s="17">
         <v>0</v>
       </c>
-      <c r="D44" s="17"/>
+      <c r="D44" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E44" s="19"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
@@ -30769,7 +30905,9 @@
       <c r="C45" s="17">
         <v>0</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E45" s="19"/>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
@@ -30788,7 +30926,9 @@
       <c r="C46" s="17">
         <v>0</v>
       </c>
-      <c r="D46" s="17"/>
+      <c r="D46" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E46" s="19"/>
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
@@ -30807,7 +30947,9 @@
       <c r="C47" s="17">
         <v>0</v>
       </c>
-      <c r="D47" s="17"/>
+      <c r="D47" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E47" s="19"/>
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
@@ -30826,7 +30968,9 @@
       <c r="C48" s="17">
         <v>0</v>
       </c>
-      <c r="D48" s="17"/>
+      <c r="D48" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E48" s="19"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
@@ -30845,7 +30989,9 @@
       <c r="C49" s="17">
         <v>0</v>
       </c>
-      <c r="D49" s="17"/>
+      <c r="D49" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E49" s="19"/>
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
@@ -30864,7 +31010,9 @@
       <c r="C50" s="17">
         <v>0</v>
       </c>
-      <c r="D50" s="17"/>
+      <c r="D50" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E50" s="19"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -30883,7 +31031,9 @@
       <c r="C51" s="17">
         <v>0</v>
       </c>
-      <c r="D51" s="17"/>
+      <c r="D51" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E51" s="19"/>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
@@ -30902,7 +31052,9 @@
       <c r="C52" s="17">
         <v>0</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E52" s="19"/>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
@@ -30921,7 +31073,9 @@
       <c r="C53" s="17">
         <v>0</v>
       </c>
-      <c r="D53" s="17"/>
+      <c r="D53" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E53" s="19"/>
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
@@ -30940,7 +31094,9 @@
       <c r="C54" s="17">
         <v>0</v>
       </c>
-      <c r="D54" s="17"/>
+      <c r="D54" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E54" s="19"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -30959,7 +31115,9 @@
       <c r="C55" s="17">
         <v>0</v>
       </c>
-      <c r="D55" s="17"/>
+      <c r="D55" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E55" s="19"/>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -30978,7 +31136,9 @@
       <c r="C56" s="17">
         <v>0</v>
       </c>
-      <c r="D56" s="17"/>
+      <c r="D56" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E56" s="19"/>
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
@@ -30997,7 +31157,9 @@
       <c r="C57" s="17">
         <v>0</v>
       </c>
-      <c r="D57" s="17"/>
+      <c r="D57" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E57" s="19"/>
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
@@ -31016,7 +31178,9 @@
       <c r="C58" s="17">
         <v>0</v>
       </c>
-      <c r="D58" s="17"/>
+      <c r="D58" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E58" s="19"/>
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
@@ -31035,7 +31199,9 @@
       <c r="C59" s="17">
         <v>0</v>
       </c>
-      <c r="D59" s="17"/>
+      <c r="D59" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E59" s="19"/>
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
@@ -31054,7 +31220,9 @@
       <c r="C60" s="17">
         <v>0</v>
       </c>
-      <c r="D60" s="17"/>
+      <c r="D60" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E60" s="19"/>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
@@ -31073,7 +31241,9 @@
       <c r="C61" s="17">
         <v>0</v>
       </c>
-      <c r="D61" s="17"/>
+      <c r="D61" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E61" s="19"/>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
@@ -31092,7 +31262,9 @@
       <c r="C62" s="17">
         <v>0</v>
       </c>
-      <c r="D62" s="17"/>
+      <c r="D62" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E62" s="19"/>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
@@ -31111,7 +31283,9 @@
       <c r="C63" s="17">
         <v>0</v>
       </c>
-      <c r="D63" s="17"/>
+      <c r="D63" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="E63" s="19"/>
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>

</xml_diff>

<commit_message>
add autogen state decoding
</commit_message>
<xml_diff>
--- a/HW2/autogen/CUSignals.xlsx
+++ b/HW2/autogen/CUSignals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW2\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9378F40-1EA0-4FD5-9D64-3CD89CB7D43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEDE076-3348-49DB-9BAE-A08DD04844A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="REG" sheetId="5" r:id="rId5"/>
     <sheet name="IO" sheetId="6" r:id="rId6"/>
     <sheet name="CU" sheetId="7" r:id="rId7"/>
+    <sheet name="states" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3643" uniqueCount="274">
   <si>
     <t>Instruction</t>
   </si>
@@ -865,12 +866,34 @@
   <si>
     <t>MemWE3</t>
   </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <r>
+      <t>ALUOp</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASel</t>
+    </r>
+  </si>
+  <si>
+    <t>TRAPA_Init</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +945,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -961,7 +1007,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1000,11 +1046,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1097,11 +1154,49 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1468,34 +1563,34 @@
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="RegA1SelCmd"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="RegA2SelCmd"/>
     <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="RegOpSel"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="MemRE0" dataDxfId="15">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="MemRE0" dataDxfId="17">
       <calculatedColumnFormula>IO!B2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="MemRE1" totalsRowFunction="sum">
       <calculatedColumnFormula>IO!C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{AA866E55-9833-4C4C-9A99-7BFC73085005}" name="MemRE2" dataDxfId="14">
+    <tableColumn id="37" xr3:uid="{AA866E55-9833-4C4C-9A99-7BFC73085005}" name="MemRE2" dataDxfId="16">
       <calculatedColumnFormula>IO!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{4192AEBC-3B81-49CC-92B8-62D42F11CA95}" name="MemRE3" dataDxfId="13">
+    <tableColumn id="36" xr3:uid="{4192AEBC-3B81-49CC-92B8-62D42F11CA95}" name="MemRE3" dataDxfId="15">
       <calculatedColumnFormula>IO!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{7CC31D84-B237-4D44-A659-0C7405E0DC1D}" name="MemWE0" dataDxfId="12">
+    <tableColumn id="40" xr3:uid="{7CC31D84-B237-4D44-A659-0C7405E0DC1D}" name="MemWE0" dataDxfId="14">
       <calculatedColumnFormula>IO!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{15C72638-8A56-43C2-9285-4F3468272C8C}" name="MemWE1" dataDxfId="11">
+    <tableColumn id="39" xr3:uid="{15C72638-8A56-43C2-9285-4F3468272C8C}" name="MemWE1" dataDxfId="13">
       <calculatedColumnFormula>IO!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{F3D5076E-751D-4100-A3DF-29C6117920BB}" name="MemWE2" dataDxfId="10">
+    <tableColumn id="38" xr3:uid="{F3D5076E-751D-4100-A3DF-29C6117920BB}" name="MemWE2" dataDxfId="12">
       <calculatedColumnFormula>IO!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{DE2CE0F0-BCB6-4C57-9F42-F491574A149E}" name="MemWE3" dataDxfId="9">
+    <tableColumn id="35" xr3:uid="{DE2CE0F0-BCB6-4C57-9F42-F491574A149E}" name="MemWE3" dataDxfId="11">
       <calculatedColumnFormula>IO!I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{47C8206D-138D-4DDB-A699-0197A19A0B4B}" name="ABOutSel" dataDxfId="8">
+    <tableColumn id="34" xr3:uid="{47C8206D-138D-4DDB-A699-0197A19A0B4B}" name="ABOutSel" dataDxfId="10">
       <calculatedColumnFormula>IO!J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{3C874C55-14EC-40FD-8E1B-959A171C140E}" name="DBOutSel" dataDxfId="7">
+    <tableColumn id="33" xr3:uid="{3C874C55-14EC-40FD-8E1B-959A171C140E}" name="DBOutSel" dataDxfId="9">
       <calculatedColumnFormula>IO!K2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="NextState"/>
@@ -1577,15 +1672,15 @@
   <autoFilter ref="A1:K124" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Instruction"/>
-    <tableColumn id="8" xr3:uid="{708E7D7C-C6D1-479F-902D-CF78BF1AF9A2}" name="MemRE0" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{6D14338A-34B2-4ACD-B190-A1DB2CB86EC9}" name="MemRE1" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{0DF91437-E1C1-4E52-9413-CD9D4D7722F9}" name="MemRE2" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{708E7D7C-C6D1-479F-902D-CF78BF1AF9A2}" name="MemRE0" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{6D14338A-34B2-4ACD-B190-A1DB2CB86EC9}" name="MemRE1" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0DF91437-E1C1-4E52-9413-CD9D4D7722F9}" name="MemRE2" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="MemRE3"/>
-    <tableColumn id="11" xr3:uid="{6659E729-599B-40EA-A8B0-F8498DEDF371}" name="MemWE0" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{26C274F0-CD81-4608-80E1-ED5DE06102BE}" name="MemWE1" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{7AEE87F6-BA73-492C-80D1-B002B89E63E2}" name="MemWE2" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{6659E729-599B-40EA-A8B0-F8498DEDF371}" name="MemWE0" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{26C274F0-CD81-4608-80E1-ED5DE06102BE}" name="MemWE1" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{7AEE87F6-BA73-492C-80D1-B002B89E63E2}" name="MemWE2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="MemWE3"/>
-    <tableColumn id="5" xr3:uid="{1500673A-35D1-4BFD-8F56-96677211AC82}" name="ABOutSel" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{1500673A-35D1-4BFD-8F56-96677211AC82}" name="ABOutSel" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="DBOutSel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1599,6 +1694,55 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Instruction"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="NextState"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="UpdateIR"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}" name="Table8" displayName="Table8" ref="A1:AN5" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:AN5" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}"/>
+  <tableColumns count="40">
+    <tableColumn id="1" xr3:uid="{F3731410-185C-4B91-8535-E7C6B1BA41A0}" name="State" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{65E65804-6476-498A-9301-353C7895D8C6}" name="ALUOpASel"/>
+    <tableColumn id="3" xr3:uid="{DF2A1A99-B208-4185-89E1-C4FCCE774BB4}" name="ALUOpBSel"/>
+    <tableColumn id="4" xr3:uid="{A9D5AA0C-6DF1-42E8-9CD2-66AA8AEED612}" name="FCmd"/>
+    <tableColumn id="5" xr3:uid="{DACF35B0-F3BC-4FEC-A865-45828AF5E85E}" name="CinCmd"/>
+    <tableColumn id="6" xr3:uid="{2DA5F137-C2D2-41D8-8626-C4790BDE7667}" name="SCmd"/>
+    <tableColumn id="7" xr3:uid="{DC7DD80B-D2CA-4F3C-A039-B76DA6D20817}" name="ALUCmd"/>
+    <tableColumn id="8" xr3:uid="{BEBFCD76-ED8E-48E0-87B7-8E09D94556C8}" name="TbitOp"/>
+    <tableColumn id="9" xr3:uid="{F71F9255-478F-481C-A66B-E1954CE2C24F}" name="UpdateTbit"/>
+    <tableColumn id="10" xr3:uid="{D03E7C40-A72F-4B7A-8A35-C557B85FD4E5}" name="PAU_SrcSel"/>
+    <tableColumn id="11" xr3:uid="{FF4B496E-1266-4DF9-A2D8-224FA372D50E}" name="PAU_OffsetSel"/>
+    <tableColumn id="12" xr3:uid="{20F43386-E748-4242-8E9E-ED14DC81DAF7}" name="PAU_UpdatePC"/>
+    <tableColumn id="13" xr3:uid="{488F9CE7-AD7A-47E2-A64D-559FD4AC5647}" name="PAU_UpdatePR"/>
+    <tableColumn id="14" xr3:uid="{3AD80B3D-1D59-482B-8D89-CAD305FC9A0D}" name="DAU_SrcSel"/>
+    <tableColumn id="15" xr3:uid="{2B1D3CA2-7125-4D6F-89B7-19AD06D98F5C}" name="DAU_OffsetSel"/>
+    <tableColumn id="16" xr3:uid="{FB732868-706C-48F2-A8F9-9A08F3E67A3B}" name="DAU_IncDecSel"/>
+    <tableColumn id="17" xr3:uid="{4D6F346E-A683-45CF-AAA9-F5BD61C94368}" name="DAU_IncDecBit"/>
+    <tableColumn id="18" xr3:uid="{647034A4-E7A3-4B85-B180-C3FD71CEAAC7}" name="DAU_PrePostSel"/>
+    <tableColumn id="19" xr3:uid="{2C05416C-4735-4192-945C-373328442345}" name="DAU_LoadGBR"/>
+    <tableColumn id="20" xr3:uid="{8C5F6243-264D-404B-9125-691103C80EAC}" name="RegInSelCmd"/>
+    <tableColumn id="21" xr3:uid="{CD20F6B8-0AB9-4EEB-AE5A-B1DF50E9A13C}" name="RegStore"/>
+    <tableColumn id="22" xr3:uid="{87CBD4A5-85D9-422F-9062-6F4760DEB967}" name="RegASelCmd"/>
+    <tableColumn id="23" xr3:uid="{B42A6BC9-F429-4017-A06D-B2B8B8762DC2}" name="RegBSelCmd"/>
+    <tableColumn id="24" xr3:uid="{7B9F6AFF-11D8-4EAC-A778-EC2854339B0E}" name="RegAxInSelCmd"/>
+    <tableColumn id="25" xr3:uid="{8CA5B1B7-BE8A-4462-B7CB-B411BE2341BC}" name="RegAxStore"/>
+    <tableColumn id="26" xr3:uid="{11836704-2B70-45DA-891A-B1F64640B548}" name="RegA1SelCmd"/>
+    <tableColumn id="27" xr3:uid="{47911AB8-C6EE-45DA-81FE-9F39B90B419B}" name="RegA2SelCmd"/>
+    <tableColumn id="28" xr3:uid="{A677ABFF-93CA-456C-ACAF-13741A9E3652}" name="RegOpSel"/>
+    <tableColumn id="29" xr3:uid="{333B3F2E-5164-4E8B-BC05-677DF42BE5C4}" name="MemRE0"/>
+    <tableColumn id="30" xr3:uid="{E43E2060-A755-494E-9BBD-55290C4F8E61}" name="MemRE1"/>
+    <tableColumn id="31" xr3:uid="{8F8A568D-55B9-4C4E-A6FE-B85127B76FB6}" name="MemRE2"/>
+    <tableColumn id="32" xr3:uid="{2DBDA554-00D2-4966-8B4C-018E5EC6FCAD}" name="MemRE3"/>
+    <tableColumn id="33" xr3:uid="{7420F2D2-239C-485D-B113-5AE3BFE02B69}" name="MemWE0"/>
+    <tableColumn id="34" xr3:uid="{B285FB56-A946-4E8B-9F37-27E9FC5ED285}" name="MemWE1"/>
+    <tableColumn id="35" xr3:uid="{C08BC861-D8CB-43AA-8D55-AF1F64C8F6B4}" name="MemWE2"/>
+    <tableColumn id="36" xr3:uid="{00938648-BF7F-4F94-9769-D5224E9F58C2}" name="MemWE3"/>
+    <tableColumn id="37" xr3:uid="{A629FB90-194D-493F-945C-31F795D6209C}" name="ABOutSel"/>
+    <tableColumn id="38" xr3:uid="{C78D366F-C0E8-4AC0-81DC-095A5844FDA0}" name="DBOutSel"/>
+    <tableColumn id="39" xr3:uid="{87F6F299-68E7-4D44-B6B3-0C08EA9E8BA5}" name="NextState"/>
+    <tableColumn id="40" xr3:uid="{22D78025-FDB5-4623-8A2C-26E4D1B1C0D0}" name="UpdateIR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1894,9 +2038,9 @@
   </sheetPr>
   <dimension ref="A1:AN124"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH11" sqref="AH11"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34309,7 +34453,7 @@
   </sheetPr>
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -40801,4 +40945,418 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521BB4-2DEC-48BF-9F68-8BCAEB743C1F}">
+  <dimension ref="A1:AN3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" customWidth="1"/>
+    <col min="22" max="22" width="14" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" customWidth="1"/>
+    <col min="26" max="27" width="15.140625" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
+    <col min="29" max="32" width="10.85546875" customWidth="1"/>
+    <col min="33" max="36" width="11.5703125" customWidth="1"/>
+    <col min="37" max="38" width="11.28515625" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" customWidth="1"/>
+    <col min="40" max="40" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="S1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="U1" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z1" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB1" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC1" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD1" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE1" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="AF1" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="AG1" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AH1" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="AI1" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ1" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="AK1" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="AL1" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" t="s">
+        <v>154</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>139</v>
+      </c>
+      <c r="W2" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" t="s">
+        <v>154</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>139</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>139</v>
+      </c>
+      <c r="W3" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add swap and xtrct
</commit_message>
<xml_diff>
--- a/HW2/autogen/CUSignals.xlsx
+++ b/HW2/autogen/CUSignals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW2\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C227D46-1B76-4E7C-B31B-463C5CC4524B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA61BC1B-E43C-4C91-A411-7CCDC5F8F701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="334">
   <si>
     <t>Instruction</t>
   </si>
@@ -1045,6 +1045,15 @@
   </si>
   <si>
     <t>RegOp_EXTUW</t>
+  </si>
+  <si>
+    <t>RegOp_SWAPB</t>
+  </si>
+  <si>
+    <t>RegOp_SWAPW</t>
+  </si>
+  <si>
+    <t>RegOp_XTRCT</t>
   </si>
 </sst>
 </file>
@@ -8799,7 +8808,7 @@
       </c>
       <c r="AE38" s="16" t="str">
         <f>REG!J38</f>
-        <v>RegOp_None</v>
+        <v>RegOp_SWAPB</v>
       </c>
       <c r="AF38" s="16" t="str">
         <f>REG!K38</f>
@@ -8827,7 +8836,7 @@
       </c>
       <c r="AL38" s="16" t="str">
         <f>IO!G38</f>
-        <v>DataAccessMode_Byte</v>
+        <v>DataAccessMode_Word</v>
       </c>
       <c r="AM38" t="str">
         <f>CU!B38</f>
@@ -8973,7 +8982,7 @@
       </c>
       <c r="AE39" s="16" t="str">
         <f>REG!J39</f>
-        <v>RegOp_None</v>
+        <v>RegOp_SWAPW</v>
       </c>
       <c r="AF39" s="16" t="str">
         <f>REG!K39</f>
@@ -9147,7 +9156,7 @@
       </c>
       <c r="AE40" s="16" t="str">
         <f>REG!J40</f>
-        <v>RegOp_None</v>
+        <v>RegOp_XTRCT</v>
       </c>
       <c r="AF40" s="16" t="str">
         <f>REG!K40</f>
@@ -9175,7 +9184,7 @@
       </c>
       <c r="AL40" s="16" t="str">
         <f>IO!G40</f>
-        <v>DataAccessMode_Long</v>
+        <v>DataAccessMode_Word</v>
       </c>
       <c r="AM40" t="str">
         <f>CU!B40</f>
@@ -11649,7 +11658,7 @@
       </c>
       <c r="D55" s="17" t="str">
         <f>ALU!D55</f>
-        <v>FCmd_A</v>
+        <v>FCmd_B</v>
       </c>
       <c r="E55" s="17" t="str">
         <f>ALU!E55</f>
@@ -11823,7 +11832,7 @@
       </c>
       <c r="D56" s="17" t="str">
         <f>ALU!D56</f>
-        <v>FCmd_A</v>
+        <v>FCmd_B</v>
       </c>
       <c r="E56" s="17" t="str">
         <f>ALU!E56</f>
@@ -11997,7 +12006,7 @@
       </c>
       <c r="D57" s="17" t="str">
         <f>ALU!D57</f>
-        <v>FCmd_A</v>
+        <v>FCmd_B</v>
       </c>
       <c r="E57" s="17" t="str">
         <f>ALU!E57</f>
@@ -12171,7 +12180,7 @@
       </c>
       <c r="D58" s="17" t="str">
         <f>ALU!D58</f>
-        <v>FCmd_A</v>
+        <v>FCmd_B</v>
       </c>
       <c r="E58" s="17" t="str">
         <f>ALU!E58</f>
@@ -24004,8 +24013,8 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25599,7 +25608,7 @@
         <v>193</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>153</v>
@@ -25628,7 +25637,7 @@
         <v>193</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>153</v>
@@ -25657,7 +25666,7 @@
         <v>193</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>153</v>
@@ -25686,7 +25695,7 @@
         <v>193</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>153</v>
@@ -33826,8 +33835,8 @@
   </sheetPr>
   <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView topLeftCell="A30" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35168,7 +35177,7 @@
         <v>139</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>140</v>
+        <v>331</v>
       </c>
       <c r="K38" t="s">
         <v>288</v>
@@ -35203,7 +35212,7 @@
         <v>139</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>140</v>
+        <v>332</v>
       </c>
       <c r="K39" t="s">
         <v>288</v>
@@ -35238,7 +35247,7 @@
         <v>139</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>140</v>
+        <v>333</v>
       </c>
       <c r="K40" t="s">
         <v>288</v>
@@ -38042,7 +38051,7 @@
   <dimension ref="A1:M125"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="94" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39148,7 +39157,7 @@
       </c>
       <c r="F38" s="16"/>
       <c r="G38" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
@@ -39202,7 +39211,7 @@
       </c>
       <c r="F40" s="16"/>
       <c r="G40" s="33" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>

</xml_diff>

<commit_message>
add multi-clock logic inst
</commit_message>
<xml_diff>
--- a/HW2/autogen/CUSignals.xlsx
+++ b/HW2/autogen/CUSignals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW2\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA61BC1B-E43C-4C91-A411-7CCDC5F8F701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327F23B7-12C8-4BC9-9154-C65DC970122A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5125" uniqueCount="339">
   <si>
     <t>Instruction</t>
   </si>
@@ -1055,6 +1055,21 @@
   <si>
     <t>RegOp_XTRCT</t>
   </si>
+  <si>
+    <t>WriteBack</t>
+  </si>
+  <si>
+    <t>TempRegSel_Result</t>
+  </si>
+  <si>
+    <t>ALUOpASel_TempReg</t>
+  </si>
+  <si>
+    <t>ALUOpBSel_TASMask</t>
+  </si>
+  <si>
+    <t>Tbit_TAS</t>
+  </si>
 </sst>
 </file>
 
@@ -1215,7 +1230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1319,6 +1334,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1902,8 +1918,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}" name="Table8" displayName="Table8" ref="A1:AO8" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:AO8" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}" name="Table8" displayName="Table8" ref="A1:AO9" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:AO9" xr:uid="{BB920BEE-E24A-4706-B6A0-3848D7D63FBF}"/>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{F3731410-185C-4B91-8535-E7C6B1BA41A0}" name="State" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{65E65804-6476-498A-9301-353C7895D8C6}" name="ALUOpASel"/>
@@ -13620,23 +13636,23 @@
       </c>
       <c r="P66" s="17" t="str">
         <f>DAU!B66</f>
-        <v>unused</v>
+        <v>DAU_AddrGBR</v>
       </c>
       <c r="Q66" s="17" t="str">
         <f>DAU!C66</f>
-        <v>unused</v>
-      </c>
-      <c r="R66" s="16">
+        <v>DAU_OffsetR0</v>
+      </c>
+      <c r="R66" s="16" t="str">
         <f>DAU!D66</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="S66" s="16" t="str">
         <f>DAU!E66</f>
         <v>unused</v>
       </c>
-      <c r="T66" s="16">
+      <c r="T66" s="16" t="str">
         <f>DAU!F66</f>
-        <v>0</v>
+        <v>MemUnit_POST</v>
       </c>
       <c r="U66" s="16" t="str">
         <f>DAU!G66</f>
@@ -13660,7 +13676,7 @@
       </c>
       <c r="Z66" s="16" t="str">
         <f>REG!E66</f>
-        <v>RegBSelCmd_Rm</v>
+        <v>RegBSelCmd_R0</v>
       </c>
       <c r="AA66" s="16" t="str">
         <f>REG!F66</f>
@@ -13696,7 +13712,7 @@
       </c>
       <c r="AI66" s="16" t="str">
         <f>IO!D66</f>
-        <v>ABOutSel_Prog</v>
+        <v>ABOutSel_Data</v>
       </c>
       <c r="AJ66" s="16" t="str">
         <f>IO!E66</f>
@@ -13708,23 +13724,23 @@
       </c>
       <c r="AL66" s="16" t="str">
         <f>IO!G66</f>
-        <v>DataAccessMode_Word</v>
+        <v>DataAccessMode_Byte</v>
       </c>
       <c r="AM66" t="str">
         <f>CU!B66</f>
-        <v>Normal</v>
+        <v>WriteBack</v>
       </c>
       <c r="AN66" s="31">
         <f>CU!C66</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO66" s="16">
         <f>CU!D66</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP66" s="16" t="str">
         <f>CU!E66</f>
-        <v>unused</v>
+        <v>TempRegSel_Result</v>
       </c>
       <c r="AQ66" s="16" t="str">
         <f>CU!F66</f>
@@ -14316,23 +14332,23 @@
       </c>
       <c r="P70" s="17" t="str">
         <f>DAU!B70</f>
-        <v>unused</v>
+        <v>DAU_AddrGBR</v>
       </c>
       <c r="Q70" s="17" t="str">
         <f>DAU!C70</f>
-        <v>unused</v>
-      </c>
-      <c r="R70" s="16">
+        <v>DAU_OffsetR0</v>
+      </c>
+      <c r="R70" s="16" t="str">
         <f>DAU!D70</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="S70" s="16" t="str">
         <f>DAU!E70</f>
         <v>unused</v>
       </c>
-      <c r="T70" s="16">
+      <c r="T70" s="16" t="str">
         <f>DAU!F70</f>
-        <v>0</v>
+        <v>MemUnit_POST</v>
       </c>
       <c r="U70" s="16" t="str">
         <f>DAU!G70</f>
@@ -14356,7 +14372,7 @@
       </c>
       <c r="Z70" s="16" t="str">
         <f>REG!E70</f>
-        <v>RegBSelCmd_Rm</v>
+        <v>RegBSelCmd_R0</v>
       </c>
       <c r="AA70" s="16" t="str">
         <f>REG!F70</f>
@@ -14392,7 +14408,7 @@
       </c>
       <c r="AI70" s="16" t="str">
         <f>IO!D70</f>
-        <v>ABOutSel_Prog</v>
+        <v>ABOutSel_Data</v>
       </c>
       <c r="AJ70" s="16" t="str">
         <f>IO!E70</f>
@@ -14404,23 +14420,23 @@
       </c>
       <c r="AL70" s="16" t="str">
         <f>IO!G70</f>
-        <v>DataAccessMode_Word</v>
+        <v>DataAccessMode_Byte</v>
       </c>
       <c r="AM70" t="str">
         <f>CU!B70</f>
-        <v>Normal</v>
+        <v>WriteBack</v>
       </c>
       <c r="AN70" s="31">
         <f>CU!C70</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO70" s="16">
         <f>CU!D70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP70" s="16" t="str">
         <f>CU!E70</f>
-        <v>unused</v>
+        <v>TempRegSel_Result</v>
       </c>
       <c r="AQ70" s="16" t="str">
         <f>CU!F70</f>
@@ -14438,11 +14454,11 @@
       </c>
       <c r="C71" s="17" t="str">
         <f>ALU!C71</f>
-        <v>ALUOpBSel_RegB</v>
+        <v>ALUOpBSel_TASMask</v>
       </c>
       <c r="D71" s="17" t="str">
         <f>ALU!D71</f>
-        <v>FCmd_ONE</v>
+        <v>FCmd_OR</v>
       </c>
       <c r="E71" s="17" t="str">
         <f>ALU!E71</f>
@@ -14458,7 +14474,7 @@
       </c>
       <c r="H71" s="17" t="str">
         <f>ALU!H71</f>
-        <v>Tbit_Zero</v>
+        <v>Tbit_TAS</v>
       </c>
       <c r="I71" s="16">
         <f>ALU!I71</f>
@@ -14490,23 +14506,23 @@
       </c>
       <c r="P71" s="17" t="str">
         <f>DAU!B71</f>
-        <v>unused</v>
+        <v>DAU_AddrRn</v>
       </c>
       <c r="Q71" s="17" t="str">
         <f>DAU!C71</f>
-        <v>unused</v>
-      </c>
-      <c r="R71" s="16">
+        <v>DAU_OffsetZero</v>
+      </c>
+      <c r="R71" s="16" t="str">
         <f>DAU!D71</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="S71" s="16" t="str">
         <f>DAU!E71</f>
         <v>unused</v>
       </c>
-      <c r="T71" s="16">
+      <c r="T71" s="16" t="str">
         <f>DAU!F71</f>
-        <v>0</v>
+        <v>MemUnit_POST</v>
       </c>
       <c r="U71" s="16" t="str">
         <f>DAU!G71</f>
@@ -14526,11 +14542,11 @@
       </c>
       <c r="Y71" s="16" t="str">
         <f>REG!D71</f>
-        <v>RegASelCmd_Rn</v>
+        <v>RegASelCmd_R0</v>
       </c>
       <c r="Z71" s="16" t="str">
         <f>REG!E71</f>
-        <v>RegBSelCmd_Rm</v>
+        <v>RegBSelCmd_R0</v>
       </c>
       <c r="AA71" s="16" t="str">
         <f>REG!F71</f>
@@ -14566,7 +14582,7 @@
       </c>
       <c r="AI71" s="16" t="str">
         <f>IO!D71</f>
-        <v>ABOutSel_Prog</v>
+        <v>ABOutSel_Data</v>
       </c>
       <c r="AJ71" s="16" t="str">
         <f>IO!E71</f>
@@ -14578,23 +14594,23 @@
       </c>
       <c r="AL71" s="16" t="str">
         <f>IO!G71</f>
-        <v>DataAccessMode_Word</v>
+        <v>DataAccessMode_Byte</v>
       </c>
       <c r="AM71" t="str">
         <f>CU!B71</f>
-        <v>Normal</v>
+        <v>WriteBack</v>
       </c>
       <c r="AN71" s="31">
         <f>CU!C71</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO71" s="16">
         <f>CU!D71</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP71" s="16" t="str">
         <f>CU!E71</f>
-        <v>unused</v>
+        <v>TempRegSel_Result</v>
       </c>
       <c r="AQ71" s="16" t="str">
         <f>CU!F71</f>
@@ -15012,23 +15028,23 @@
       </c>
       <c r="P74" s="17" t="str">
         <f>DAU!B74</f>
-        <v>unused</v>
+        <v>DAU_AddrGBR</v>
       </c>
       <c r="Q74" s="17" t="str">
         <f>DAU!C74</f>
-        <v>unused</v>
-      </c>
-      <c r="R74" s="16">
+        <v>DAU_OffsetR0</v>
+      </c>
+      <c r="R74" s="16" t="str">
         <f>DAU!D74</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="S74" s="16" t="str">
         <f>DAU!E74</f>
         <v>unused</v>
       </c>
-      <c r="T74" s="16">
+      <c r="T74" s="16" t="str">
         <f>DAU!F74</f>
-        <v>0</v>
+        <v>MemUnit_POST</v>
       </c>
       <c r="U74" s="16" t="str">
         <f>DAU!G74</f>
@@ -15052,7 +15068,7 @@
       </c>
       <c r="Z74" s="16" t="str">
         <f>REG!E74</f>
-        <v>RegBSelCmd_Rm</v>
+        <v>RegBSelCmd_R0</v>
       </c>
       <c r="AA74" s="16" t="str">
         <f>REG!F74</f>
@@ -15088,7 +15104,7 @@
       </c>
       <c r="AI74" s="16" t="str">
         <f>IO!D74</f>
-        <v>ABOutSel_Prog</v>
+        <v>ABOutSel_Data</v>
       </c>
       <c r="AJ74" s="16" t="str">
         <f>IO!E74</f>
@@ -15100,23 +15116,23 @@
       </c>
       <c r="AL74" s="16" t="str">
         <f>IO!G74</f>
-        <v>DataAccessMode_Word</v>
+        <v>DataAccessMode_Byte</v>
       </c>
       <c r="AM74" t="str">
         <f>CU!B74</f>
-        <v>Normal</v>
+        <v>WaitForFetch</v>
       </c>
       <c r="AN74" s="31">
         <f>CU!C74</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO74" s="16">
         <f>CU!D74</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP74" s="16" t="str">
         <f>CU!E74</f>
-        <v>unused</v>
+        <v>TempRegSel_Result</v>
       </c>
       <c r="AQ74" s="16" t="str">
         <f>CU!F74</f>
@@ -15478,7 +15494,7 @@
       </c>
       <c r="B77" s="17" t="str">
         <f>ALU!B77</f>
-        <v>ALUOpASel_RegA</v>
+        <v>ALUOpASel_DB</v>
       </c>
       <c r="C77" s="17" t="str">
         <f>ALU!C77</f>
@@ -15534,23 +15550,23 @@
       </c>
       <c r="P77" s="17" t="str">
         <f>DAU!B77</f>
-        <v>unused</v>
+        <v>DAU_AddrGBR</v>
       </c>
       <c r="Q77" s="17" t="str">
         <f>DAU!C77</f>
-        <v>unused</v>
-      </c>
-      <c r="R77" s="16">
+        <v>DAU_OffsetR0</v>
+      </c>
+      <c r="R77" s="16" t="str">
         <f>DAU!D77</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="S77" s="16" t="str">
         <f>DAU!E77</f>
         <v>unused</v>
       </c>
-      <c r="T77" s="16">
+      <c r="T77" s="16" t="str">
         <f>DAU!F77</f>
-        <v>0</v>
+        <v>MemUnit_POST</v>
       </c>
       <c r="U77" s="16" t="str">
         <f>DAU!G77</f>
@@ -15574,7 +15590,7 @@
       </c>
       <c r="Z77" s="16" t="str">
         <f>REG!E77</f>
-        <v>RegBSelCmd_Rm</v>
+        <v>RegBSelCmd_R0</v>
       </c>
       <c r="AA77" s="16" t="str">
         <f>REG!F77</f>
@@ -15610,7 +15626,7 @@
       </c>
       <c r="AI77" s="16" t="str">
         <f>IO!D77</f>
-        <v>ABOutSel_Prog</v>
+        <v>ABOutSel_Data</v>
       </c>
       <c r="AJ77" s="16" t="str">
         <f>IO!E77</f>
@@ -15622,23 +15638,23 @@
       </c>
       <c r="AL77" s="16" t="str">
         <f>IO!G77</f>
-        <v>DataAccessMode_Word</v>
+        <v>DataAccessMode_Byte</v>
       </c>
       <c r="AM77" t="str">
         <f>CU!B77</f>
-        <v>Normal</v>
+        <v>WriteBack</v>
       </c>
       <c r="AN77" s="31">
         <f>CU!C77</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO77" s="16">
         <f>CU!D77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP77" s="16" t="str">
         <f>CU!E77</f>
-        <v>unused</v>
+        <v>TempRegSel_Result</v>
       </c>
       <c r="AQ77" s="16" t="str">
         <f>CU!F77</f>
@@ -24013,8 +24029,8 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26068,11 +26084,11 @@
       <c r="B71" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C71" s="19" t="s">
-        <v>193</v>
+      <c r="C71" s="17" t="s">
+        <v>337</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E71" s="17" t="s">
         <v>153</v>
@@ -26084,7 +26100,7 @@
         <v>191</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>202</v>
+        <v>338</v>
       </c>
       <c r="I71" s="20">
         <v>1</v>
@@ -26239,8 +26255,8 @@
       <c r="A77" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>192</v>
+      <c r="B77" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>215</v>
@@ -27671,7 +27687,7 @@
   </sheetPr>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -30577,8 +30593,8 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32288,16 +32304,20 @@
         <v>67</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D66" s="17"/>
+        <v>166</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E66" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F66" s="18"/>
+      <c r="F66" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="G66" s="24" t="s">
         <v>311</v>
       </c>
@@ -32388,16 +32408,20 @@
         <v>71</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D70" s="17"/>
+        <v>166</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E70" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F70" s="18"/>
+      <c r="F70" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="G70" s="24" t="s">
         <v>311</v>
       </c>
@@ -32410,16 +32434,20 @@
         <v>72</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D71" s="17"/>
+        <v>159</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E71" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F71" s="18"/>
+      <c r="F71" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="G71" s="24" t="s">
         <v>311</v>
       </c>
@@ -32484,16 +32512,20 @@
         <v>75</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D74" s="17"/>
+        <v>166</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E74" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F74" s="18"/>
+      <c r="F74" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="G74" s="24" t="s">
         <v>311</v>
       </c>
@@ -32558,16 +32590,20 @@
         <v>78</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D77" s="17"/>
+        <v>166</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E77" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="18"/>
+      <c r="F77" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="G77" s="24" t="s">
         <v>311</v>
       </c>
@@ -33835,8 +33871,8 @@
   </sheetPr>
   <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="A52" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36142,7 +36178,7 @@
         <v>252</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>139</v>
@@ -36282,7 +36318,7 @@
         <v>252</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>139</v>
@@ -36314,10 +36350,10 @@
         <v>0</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F71" s="18" t="s">
         <v>139</v>
@@ -36422,7 +36458,7 @@
         <v>252</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>139</v>
@@ -36527,7 +36563,7 @@
         <v>252</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F77" s="18" t="s">
         <v>139</v>
@@ -38050,8 +38086,8 @@
   </sheetPr>
   <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="94" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A49" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39952,14 +39988,14 @@
         <v>1</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>269</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="18"/>
@@ -40060,14 +40096,14 @@
         <v>1</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>269</v>
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H70" s="19"/>
       <c r="I70" s="18"/>
@@ -40087,14 +40123,14 @@
         <v>1</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>269</v>
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H71" s="19"/>
       <c r="I71" s="18"/>
@@ -40168,14 +40204,14 @@
         <v>1</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>269</v>
       </c>
       <c r="F74" s="20"/>
       <c r="G74" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H74" s="19"/>
       <c r="I74" s="18"/>
@@ -40249,14 +40285,14 @@
         <v>1</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>269</v>
       </c>
       <c r="F77" s="20"/>
       <c r="G77" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H77" s="19"/>
       <c r="I77" s="18"/>
@@ -41532,8 +41568,8 @@
   </sheetPr>
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A61" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42850,16 +42886,16 @@
         <v>67</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C66" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="F66" t="s">
         <v>300</v>
@@ -42930,16 +42966,16 @@
         <v>71</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C70" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="F70" t="s">
         <v>300</v>
@@ -42950,16 +42986,16 @@
         <v>72</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C71" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="F71" t="s">
         <v>300</v>
@@ -43010,16 +43046,16 @@
         <v>75</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C74" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="F74" t="s">
         <v>300</v>
@@ -43070,16 +43106,16 @@
         <v>78</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C77" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>139</v>
+        <v>335</v>
       </c>
       <c r="F77" t="s">
         <v>300</v>
@@ -43924,10 +43960,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521BB4-2DEC-48BF-9F68-8BCAEB743C1F}">
-  <dimension ref="A1:AO8"/>
+  <dimension ref="A1:AO9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44966,6 +45002,131 @@
         <v>156</v>
       </c>
     </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="B9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" t="s">
+        <v>271</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>271</v>
+      </c>
+      <c r="K9" t="s">
+        <v>271</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>271</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="T9" t="s">
+        <v>313</v>
+      </c>
+      <c r="U9" t="s">
+        <v>271</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>271</v>
+      </c>
+      <c r="X9" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>249</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>251</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
progress in debuggin branch mem access
</commit_message>
<xml_diff>
--- a/HW2/autogen/CUSignals.xlsx
+++ b/HW2/autogen/CUSignals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW2\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2629F1B9-3E82-432A-8ACB-8067A008F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FA5888-D4F1-4850-9CF5-2423FED9B17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5409" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5409" uniqueCount="350">
   <si>
     <t>Instruction</t>
   </si>
@@ -1110,12 +1110,15 @@
   <si>
     <t>ALUOpASel_TempReg1</t>
   </si>
+  <si>
+    <t>TempReg1Sel_PC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1162,13 @@
       <name val="Aptos Display"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1247,7 +1257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1336,11 +1346,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1615,7 +1638,7 @@
     <tableColumn id="33" xr3:uid="{00000000-0010-0000-0700-000021000000}" name="DBOutSel"/>
     <tableColumn id="34" xr3:uid="{00000000-0010-0000-0700-000022000000}" name="DataAccessMode"/>
     <tableColumn id="35" xr3:uid="{00000000-0010-0000-0700-000023000000}" name="NextState"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0700-000024000000}" name="UpdateIR"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0700-000024000000}" name="UpdateIR" dataDxfId="0"/>
     <tableColumn id="37" xr3:uid="{00000000-0010-0000-0700-000025000000}" name="UpdateTempReg1"/>
     <tableColumn id="38" xr3:uid="{00000000-0010-0000-0700-000026000000}" name="TempReg1Sel"/>
     <tableColumn id="39" xr3:uid="{00000000-0010-0000-0700-000027000000}" name="PAU_IncDecBit"/>
@@ -1806,10 +1829,10 @@
   </sheetPr>
   <dimension ref="A1:AR126"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AG1" sqref="AG1"/>
-      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1"/>
+      <selection pane="bottomLeft" activeCell="AQ101" sqref="AQ101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2205,15 +2228,15 @@
       </c>
       <c r="J3" s="7" t="str">
         <f>PAU!B3</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K3" s="7" t="str">
         <f>PAU!C3</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L3" s="8">
         <f>PAU!D3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="8" t="str">
         <f>PAU!E3</f>
@@ -2383,15 +2406,15 @@
       </c>
       <c r="J4" s="7" t="str">
         <f>PAU!B4</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K4" s="7" t="str">
         <f>PAU!C4</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L4" s="8">
         <f>PAU!D4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="8" t="str">
         <f>PAU!E4</f>
@@ -2739,15 +2762,15 @@
       </c>
       <c r="J6" s="7" t="str">
         <f>PAU!B6</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K6" s="7" t="str">
         <f>PAU!C6</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L6" s="8">
         <f>PAU!D6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="8" t="str">
         <f>PAU!E6</f>
@@ -2917,15 +2940,15 @@
       </c>
       <c r="J7" s="7" t="str">
         <f>PAU!B7</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K7" s="7" t="str">
         <f>PAU!C7</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L7" s="8">
         <f>PAU!D7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="8" t="str">
         <f>PAU!E7</f>
@@ -3095,15 +3118,15 @@
       </c>
       <c r="J8" s="7" t="str">
         <f>PAU!B8</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K8" s="7" t="str">
         <f>PAU!C8</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L8" s="8">
         <f>PAU!D8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="8" t="str">
         <f>PAU!E8</f>
@@ -3273,15 +3296,15 @@
       </c>
       <c r="J9" s="7" t="str">
         <f>PAU!B9</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K9" s="7" t="str">
         <f>PAU!C9</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L9" s="8">
         <f>PAU!D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="8" t="str">
         <f>PAU!E9</f>
@@ -3451,15 +3474,15 @@
       </c>
       <c r="J10" s="7" t="str">
         <f>PAU!B10</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K10" s="7" t="str">
         <f>PAU!C10</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L10" s="8">
         <f>PAU!D10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="8" t="str">
         <f>PAU!E10</f>
@@ -3629,15 +3652,15 @@
       </c>
       <c r="J11" s="7" t="str">
         <f>PAU!B11</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K11" s="7" t="str">
         <f>PAU!C11</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L11" s="8">
         <f>PAU!D11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="8" t="str">
         <f>PAU!E11</f>
@@ -3807,15 +3830,15 @@
       </c>
       <c r="J12" s="7" t="str">
         <f>PAU!B12</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K12" s="7" t="str">
         <f>PAU!C12</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L12" s="8">
         <f>PAU!D12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="8" t="str">
         <f>PAU!E12</f>
@@ -3985,15 +4008,15 @@
       </c>
       <c r="J13" s="7" t="str">
         <f>PAU!B13</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K13" s="7" t="str">
         <f>PAU!C13</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L13" s="8">
         <f>PAU!D13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="8" t="str">
         <f>PAU!E13</f>
@@ -4163,15 +4186,15 @@
       </c>
       <c r="J14" s="7" t="str">
         <f>PAU!B14</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K14" s="7" t="str">
         <f>PAU!C14</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L14" s="8">
         <f>PAU!D14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="8" t="str">
         <f>PAU!E14</f>
@@ -4341,15 +4364,15 @@
       </c>
       <c r="J15" s="7" t="str">
         <f>PAU!B15</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K15" s="7" t="str">
         <f>PAU!C15</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L15" s="8">
         <f>PAU!D15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="8" t="str">
         <f>PAU!E15</f>
@@ -4519,15 +4542,15 @@
       </c>
       <c r="J16" s="7" t="str">
         <f>PAU!B16</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K16" s="7" t="str">
         <f>PAU!C16</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L16" s="8">
         <f>PAU!D16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="8" t="str">
         <f>PAU!E16</f>
@@ -4697,15 +4720,15 @@
       </c>
       <c r="J17" s="7" t="str">
         <f>PAU!B17</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K17" s="7" t="str">
         <f>PAU!C17</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L17" s="8">
         <f>PAU!D17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="8" t="str">
         <f>PAU!E17</f>
@@ -4875,15 +4898,15 @@
       </c>
       <c r="J18" s="7" t="str">
         <f>PAU!B18</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K18" s="7" t="str">
         <f>PAU!C18</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L18" s="8">
         <f>PAU!D18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="8" t="str">
         <f>PAU!E18</f>
@@ -5053,15 +5076,15 @@
       </c>
       <c r="J19" s="7" t="str">
         <f>PAU!B19</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>PAU!C19</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L19" s="8">
         <f>PAU!D19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="8" t="str">
         <f>PAU!E19</f>
@@ -5231,15 +5254,15 @@
       </c>
       <c r="J20" s="7" t="str">
         <f>PAU!B20</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K20" s="7" t="str">
         <f>PAU!C20</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L20" s="8">
         <f>PAU!D20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="8" t="str">
         <f>PAU!E20</f>
@@ -5409,15 +5432,15 @@
       </c>
       <c r="J21" s="7" t="str">
         <f>PAU!B21</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K21" s="7" t="str">
         <f>PAU!C21</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L21" s="8">
         <f>PAU!D21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="8" t="str">
         <f>PAU!E21</f>
@@ -5587,15 +5610,15 @@
       </c>
       <c r="J22" s="7" t="str">
         <f>PAU!B22</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K22" s="7" t="str">
         <f>PAU!C22</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L22" s="8">
         <f>PAU!D22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="8" t="str">
         <f>PAU!E22</f>
@@ -5765,15 +5788,15 @@
       </c>
       <c r="J23" s="7" t="str">
         <f>PAU!B23</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K23" s="7" t="str">
         <f>PAU!C23</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L23" s="8">
         <f>PAU!D23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="8" t="str">
         <f>PAU!E23</f>
@@ -5943,15 +5966,15 @@
       </c>
       <c r="J24" s="7" t="str">
         <f>PAU!B24</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K24" s="7" t="str">
         <f>PAU!C24</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L24" s="8">
         <f>PAU!D24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="8" t="str">
         <f>PAU!E24</f>
@@ -6121,15 +6144,15 @@
       </c>
       <c r="J25" s="7" t="str">
         <f>PAU!B25</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K25" s="7" t="str">
         <f>PAU!C25</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L25" s="8">
         <f>PAU!D25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="8" t="str">
         <f>PAU!E25</f>
@@ -6299,15 +6322,15 @@
       </c>
       <c r="J26" s="7" t="str">
         <f>PAU!B26</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K26" s="7" t="str">
         <f>PAU!C26</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L26" s="8">
         <f>PAU!D26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="8" t="str">
         <f>PAU!E26</f>
@@ -6477,15 +6500,15 @@
       </c>
       <c r="J27" s="7" t="str">
         <f>PAU!B27</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K27" s="7" t="str">
         <f>PAU!C27</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L27" s="8">
         <f>PAU!D27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="8" t="str">
         <f>PAU!E27</f>
@@ -6655,15 +6678,15 @@
       </c>
       <c r="J28" s="7" t="str">
         <f>PAU!B28</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K28" s="7" t="str">
         <f>PAU!C28</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L28" s="8">
         <f>PAU!D28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="8" t="str">
         <f>PAU!E28</f>
@@ -6833,15 +6856,15 @@
       </c>
       <c r="J29" s="7" t="str">
         <f>PAU!B29</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K29" s="7" t="str">
         <f>PAU!C29</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L29" s="8">
         <f>PAU!D29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="8" t="str">
         <f>PAU!E29</f>
@@ -7011,15 +7034,15 @@
       </c>
       <c r="J30" s="7" t="str">
         <f>PAU!B30</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K30" s="7" t="str">
         <f>PAU!C30</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L30" s="8">
         <f>PAU!D30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="8" t="str">
         <f>PAU!E30</f>
@@ -7189,15 +7212,15 @@
       </c>
       <c r="J31" s="7" t="str">
         <f>PAU!B31</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K31" s="7" t="str">
         <f>PAU!C31</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L31" s="8">
         <f>PAU!D31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="8" t="str">
         <f>PAU!E31</f>
@@ -7367,15 +7390,15 @@
       </c>
       <c r="J32" s="7" t="str">
         <f>PAU!B32</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K32" s="7" t="str">
         <f>PAU!C32</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L32" s="8">
         <f>PAU!D32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="8" t="str">
         <f>PAU!E32</f>
@@ -7545,15 +7568,15 @@
       </c>
       <c r="J33" s="7" t="str">
         <f>PAU!B33</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K33" s="7" t="str">
         <f>PAU!C33</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L33" s="8">
         <f>PAU!D33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="8" t="str">
         <f>PAU!E33</f>
@@ -7723,15 +7746,15 @@
       </c>
       <c r="J34" s="7" t="str">
         <f>PAU!B34</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K34" s="7" t="str">
         <f>PAU!C34</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L34" s="8">
         <f>PAU!D34</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="8" t="str">
         <f>PAU!E34</f>
@@ -7901,15 +7924,15 @@
       </c>
       <c r="J35" s="7" t="str">
         <f>PAU!B35</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K35" s="7" t="str">
         <f>PAU!C35</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L35" s="8">
         <f>PAU!D35</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="8" t="str">
         <f>PAU!E35</f>
@@ -8195,11 +8218,11 @@
       </c>
       <c r="AM36" t="str">
         <f>CU!B36</f>
-        <v>Normal</v>
+        <v>WaitForFetch</v>
       </c>
       <c r="AN36" s="4">
         <f>CU!C36</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO36" s="8">
         <f>CU!D36</f>
@@ -13419,15 +13442,15 @@
       </c>
       <c r="J66" s="7" t="str">
         <f>PAU!B66</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K66" s="7" t="str">
         <f>PAU!C66</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L66" s="8">
         <f>PAU!D66</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M66" s="8" t="str">
         <f>PAU!E66</f>
@@ -14131,15 +14154,15 @@
       </c>
       <c r="J70" s="7" t="str">
         <f>PAU!B70</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K70" s="7" t="str">
         <f>PAU!C70</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L70" s="8">
         <f>PAU!D70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="8" t="str">
         <f>PAU!E70</f>
@@ -14309,15 +14332,15 @@
       </c>
       <c r="J71" s="7" t="str">
         <f>PAU!B71</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K71" s="7" t="str">
         <f>PAU!C71</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L71" s="8">
         <f>PAU!D71</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M71" s="8" t="str">
         <f>PAU!E71</f>
@@ -14843,15 +14866,15 @@
       </c>
       <c r="J74" s="7" t="str">
         <f>PAU!B74</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K74" s="7" t="str">
         <f>PAU!C74</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L74" s="8">
         <f>PAU!D74</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74" s="8" t="str">
         <f>PAU!E74</f>
@@ -15377,15 +15400,15 @@
       </c>
       <c r="J77" s="7" t="str">
         <f>PAU!B77</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K77" s="7" t="str">
         <f>PAU!C77</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L77" s="8">
         <f>PAU!D77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M77" s="8" t="str">
         <f>PAU!E77</f>
@@ -19835,7 +19858,7 @@
       </c>
       <c r="L102" s="8">
         <f>PAU!D102</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M102" s="8" t="str">
         <f>PAU!E102</f>
@@ -20717,15 +20740,15 @@
       </c>
       <c r="J107" s="7" t="str">
         <f>PAU!B107</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K107" s="7" t="str">
         <f>PAU!C107</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L107" s="8">
         <f>PAU!D107</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M107" s="8" t="str">
         <f>PAU!E107</f>
@@ -20895,15 +20918,15 @@
       </c>
       <c r="J108" s="7" t="str">
         <f>PAU!B108</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K108" s="7" t="str">
         <f>PAU!C108</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L108" s="8">
         <f>PAU!D108</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M108" s="8" t="str">
         <f>PAU!E108</f>
@@ -21073,15 +21096,15 @@
       </c>
       <c r="J109" s="7" t="str">
         <f>PAU!B109</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K109" s="7" t="str">
         <f>PAU!C109</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L109" s="8">
         <f>PAU!D109</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M109" s="8" t="str">
         <f>PAU!E109</f>
@@ -21429,15 +21452,15 @@
       </c>
       <c r="J111" s="7" t="str">
         <f>PAU!B111</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K111" s="7" t="str">
         <f>PAU!C111</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L111" s="8">
         <f>PAU!D111</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M111" s="8" t="str">
         <f>PAU!E111</f>
@@ -21963,15 +21986,15 @@
       </c>
       <c r="J114" s="7" t="str">
         <f>PAU!B114</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K114" s="7" t="str">
         <f>PAU!C114</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L114" s="8">
         <f>PAU!D114</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M114" s="8" t="str">
         <f>PAU!E114</f>
@@ -22853,15 +22876,15 @@
       </c>
       <c r="J119" s="7" t="str">
         <f>PAU!B119</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K119" s="7" t="str">
         <f>PAU!C119</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L119" s="8">
         <f>PAU!D119</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M119" s="8" t="str">
         <f>PAU!E119</f>
@@ -23031,15 +23054,15 @@
       </c>
       <c r="J120" s="7" t="str">
         <f>PAU!B120</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K120" s="7" t="str">
         <f>PAU!C120</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L120" s="8">
         <f>PAU!D120</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M120" s="8" t="str">
         <f>PAU!E120</f>
@@ -23209,15 +23232,15 @@
       </c>
       <c r="J121" s="7" t="str">
         <f>PAU!B121</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K121" s="7" t="str">
         <f>PAU!C121</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L121" s="8">
         <f>PAU!D121</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M121" s="8" t="str">
         <f>PAU!E121</f>
@@ -23573,7 +23596,7 @@
       </c>
       <c r="L123" s="8">
         <f>PAU!D123</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M123" s="8" t="str">
         <f>PAU!E123</f>
@@ -23743,15 +23766,15 @@
       </c>
       <c r="J124" s="7" t="str">
         <f>PAU!B124</f>
-        <v>unused</v>
+        <v>PAU_AddrPC</v>
       </c>
       <c r="K124" s="7" t="str">
         <f>PAU!C124</f>
-        <v>unused</v>
+        <v>PAU_OffsetWord</v>
       </c>
       <c r="L124" s="8">
         <f>PAU!D124</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M124" s="8" t="str">
         <f>PAU!E124</f>
@@ -24078,7 +24101,7 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+    <sheetView topLeftCell="A83" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -27737,8 +27760,8 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView topLeftCell="A84" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27809,13 +27832,13 @@
         <v>216</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>214</v>
@@ -27835,13 +27858,13 @@
         <v>217</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>214</v>
@@ -27887,13 +27910,13 @@
         <v>58</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>214</v>
@@ -27913,13 +27936,13 @@
         <v>59</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>214</v>
@@ -27939,13 +27962,13 @@
         <v>60</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>214</v>
@@ -27965,13 +27988,13 @@
         <v>61</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>214</v>
@@ -27991,13 +28014,13 @@
         <v>62</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>214</v>
@@ -28017,13 +28040,13 @@
         <v>63</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>214</v>
@@ -28043,13 +28066,13 @@
         <v>64</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>214</v>
@@ -28069,13 +28092,13 @@
         <v>65</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>214</v>
@@ -28095,13 +28118,13 @@
         <v>66</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>214</v>
@@ -28121,13 +28144,13 @@
         <v>67</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>214</v>
@@ -28147,13 +28170,13 @@
         <v>68</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>214</v>
@@ -28173,13 +28196,13 @@
         <v>69</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>214</v>
@@ -28199,13 +28222,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>214</v>
@@ -28225,13 +28248,13 @@
         <v>71</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>214</v>
@@ -28251,13 +28274,13 @@
         <v>72</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>214</v>
@@ -28277,13 +28300,13 @@
         <v>73</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>214</v>
@@ -28303,13 +28326,13 @@
         <v>74</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>214</v>
@@ -28329,13 +28352,13 @@
         <v>75</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>214</v>
@@ -28355,13 +28378,13 @@
         <v>76</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>214</v>
@@ -28381,13 +28404,13 @@
         <v>77</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>214</v>
@@ -28407,13 +28430,13 @@
         <v>78</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>214</v>
@@ -28433,13 +28456,13 @@
         <v>79</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>214</v>
@@ -28459,13 +28482,13 @@
         <v>80</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>214</v>
@@ -28485,13 +28508,13 @@
         <v>81</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>214</v>
@@ -28511,13 +28534,13 @@
         <v>82</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>214</v>
@@ -28537,13 +28560,13 @@
         <v>83</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>214</v>
@@ -28563,13 +28586,13 @@
         <v>84</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>214</v>
@@ -28589,13 +28612,13 @@
         <v>85</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>214</v>
@@ -28615,13 +28638,13 @@
         <v>86</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>214</v>
@@ -28641,13 +28664,13 @@
         <v>87</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>214</v>
@@ -28672,7 +28695,7 @@
       <c r="C36" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="8">
         <v>1</v>
       </c>
       <c r="E36" s="19" t="s">
@@ -29447,13 +29470,13 @@
         <v>139</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D66" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>214</v>
@@ -29551,13 +29574,13 @@
         <v>144</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D70" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>214</v>
@@ -29577,13 +29600,13 @@
         <v>145</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D71" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="19" t="s">
         <v>214</v>
@@ -29655,13 +29678,13 @@
         <v>150</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D74" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="19" t="s">
         <v>214</v>
@@ -29733,13 +29756,13 @@
         <v>154</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D77" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="19" t="s">
         <v>214</v>
@@ -30389,7 +30412,7 @@
         <v>213</v>
       </c>
       <c r="D102" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="19" t="s">
         <v>214</v>
@@ -30513,13 +30536,13 @@
         <v>192</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D107" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D107" s="8">
+        <v>1</v>
       </c>
       <c r="E107" s="19" t="s">
         <v>214</v>
@@ -30539,13 +30562,13 @@
         <v>193</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D108" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="19" t="s">
         <v>214</v>
@@ -30565,13 +30588,13 @@
         <v>194</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D109" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" s="19" t="s">
         <v>214</v>
@@ -30617,13 +30640,13 @@
         <v>196</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D111" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="19" t="s">
         <v>223</v>
@@ -30694,14 +30717,14 @@
       <c r="A114" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B114" s="18" t="s">
-        <v>51</v>
+      <c r="B114" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="D114" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" s="19" t="s">
         <v>214</v>
@@ -30825,13 +30848,13 @@
         <v>231</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D119" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D119" s="8">
+        <v>1</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>214</v>
@@ -30851,13 +30874,13 @@
         <v>232</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D120" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D120" s="8">
+        <v>1</v>
       </c>
       <c r="E120" s="19" t="s">
         <v>214</v>
@@ -30877,13 +30900,13 @@
         <v>233</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D121" s="19">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D121" s="8">
+        <v>1</v>
       </c>
       <c r="E121" s="19" t="s">
         <v>214</v>
@@ -30935,7 +30958,7 @@
         <v>213</v>
       </c>
       <c r="D123" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>214</v>
@@ -30954,14 +30977,14 @@
       <c r="A124" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="B124" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C124" s="18" t="s">
-        <v>51</v>
+      <c r="B124" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="D124" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" s="19" t="s">
         <v>214</v>
@@ -31018,7 +31041,7 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
       <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
@@ -42065,8 +42088,8 @@
   </sheetPr>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView topLeftCell="A80" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -42075,9 +42098,9 @@
     <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42890,10 +42913,10 @@
         <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -44842,8 +44865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AQ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="AH1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44876,8 +44899,8 @@
     <col min="30" max="30" width="11.5703125" customWidth="1"/>
     <col min="31" max="31" width="19.85546875" customWidth="1"/>
     <col min="32" max="33" width="11.28515625" customWidth="1"/>
-    <col min="34" max="34" width="17" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="34" max="34" width="33" customWidth="1"/>
+    <col min="35" max="35" width="34.85546875" customWidth="1"/>
     <col min="36" max="36" width="11.140625" customWidth="1"/>
     <col min="37" max="37" width="18.7109375" customWidth="1"/>
     <col min="38" max="38" width="17.7109375" customWidth="1"/>
@@ -44992,7 +45015,7 @@
       <c r="AH1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="32" t="s">
         <v>38</v>
       </c>
       <c r="AJ1" s="4" t="s">
@@ -45052,10 +45075,10 @@
         <v>212</v>
       </c>
       <c r="K2" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>214</v>
@@ -45126,7 +45149,7 @@
       <c r="AI2" t="s">
         <v>310</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="34">
         <v>1</v>
       </c>
       <c r="AK2">
@@ -45257,7 +45280,7 @@
       <c r="AI3" t="s">
         <v>321</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="34">
         <v>0</v>
       </c>
       <c r="AK3">
@@ -45386,9 +45409,9 @@
         <v>327</v>
       </c>
       <c r="AI4" t="s">
-        <v>310</v>
-      </c>
-      <c r="AJ4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AJ4" s="34" t="s">
         <v>327</v>
       </c>
       <c r="AK4">
@@ -45517,16 +45540,16 @@
         <v>327</v>
       </c>
       <c r="AI5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AJ5" t="s">
         <v>327</v>
       </c>
+      <c r="AJ5" s="34" t="s">
+        <v>327</v>
+      </c>
       <c r="AK5">
         <v>1</v>
       </c>
       <c r="AL5" t="s">
-        <v>51</v>
+        <v>349</v>
       </c>
       <c r="AM5">
         <v>0</v>
@@ -45648,16 +45671,16 @@
         <v>327</v>
       </c>
       <c r="AI6" t="s">
-        <v>310</v>
-      </c>
-      <c r="AJ6" t="s">
         <v>327</v>
       </c>
+      <c r="AJ6" s="34" t="s">
+        <v>327</v>
+      </c>
       <c r="AK6">
         <v>1</v>
       </c>
       <c r="AL6" t="s">
-        <v>51</v>
+        <v>349</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -45781,7 +45804,7 @@
       <c r="AI7" t="s">
         <v>333</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AJ7" s="34" t="s">
         <v>327</v>
       </c>
       <c r="AK7">
@@ -45912,7 +45935,7 @@
       <c r="AI8" t="s">
         <v>310</v>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="34">
         <v>1</v>
       </c>
       <c r="AK8">
@@ -46043,7 +46066,7 @@
       <c r="AI9" t="s">
         <v>312</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="34">
         <v>0</v>
       </c>
       <c r="AK9">
@@ -46168,13 +46191,13 @@
       <c r="AG10" t="s">
         <v>327</v>
       </c>
-      <c r="AH10" s="8" t="s">
+      <c r="AH10" s="33" t="s">
         <v>299</v>
       </c>
       <c r="AI10" t="s">
         <v>310</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="34">
         <v>1</v>
       </c>
       <c r="AK10" t="s">
@@ -46305,7 +46328,7 @@
       <c r="AI11" t="s">
         <v>334</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11" s="34" t="s">
         <v>327</v>
       </c>
       <c r="AK11" t="s">
@@ -46436,7 +46459,7 @@
       <c r="AI12" t="s">
         <v>335</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12" s="34" t="s">
         <v>327</v>
       </c>
       <c r="AK12" t="s">
@@ -46567,7 +46590,7 @@
       <c r="AI13" t="s">
         <v>310</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="34">
         <v>1</v>
       </c>
       <c r="AK13">
@@ -46698,7 +46721,7 @@
       <c r="AI14" t="s">
         <v>338</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="34">
         <v>1</v>
       </c>
       <c r="AK14">
@@ -46829,7 +46852,7 @@
       <c r="AI15" t="s">
         <v>339</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AJ15" s="34" t="s">
         <v>327</v>
       </c>
       <c r="AK15">

</xml_diff>